<commit_message>
Framework Config i18n good
</commit_message>
<xml_diff>
--- a/Client/DataTables/Datas/#i18n.xlsx
+++ b/Client/DataTables/Datas/#i18n.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12375"/>
+    <workbookView windowWidth="28800" windowHeight="12375" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="UI" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
   <si>
     <t>##var</t>
   </si>
@@ -41,6 +41,12 @@
   </si>
   <si>
     <t>cn</t>
+  </si>
+  <si>
+    <t>tw</t>
+  </si>
+  <si>
+    <t>jp</t>
   </si>
   <si>
     <t>##type</t>
@@ -58,6 +64,12 @@
     <t>打开</t>
   </si>
   <si>
+    <t>打開</t>
+  </si>
+  <si>
+    <t>開ける</t>
+  </si>
+  <si>
     <t>LC_UI_Close</t>
   </si>
   <si>
@@ -65,6 +77,12 @@
   </si>
   <si>
     <t>关闭</t>
+  </si>
+  <si>
+    <t>關閉</t>
+  </si>
+  <si>
+    <t>閉鎖</t>
   </si>
   <si>
     <t>LC_Mail_Reward</t>
@@ -76,6 +94,12 @@
     <t>奖励</t>
   </si>
   <si>
+    <t>獎勵</t>
+  </si>
+  <si>
+    <t>賞</t>
+  </si>
+  <si>
     <t>LC_Mail_GetAward</t>
   </si>
   <si>
@@ -83,6 +107,12 @@
   </si>
   <si>
     <t>领奖</t>
+  </si>
+  <si>
+    <t>領取</t>
+  </si>
+  <si>
+    <t>受け取る</t>
   </si>
 </sst>
 </file>
@@ -1089,8 +1119,8 @@
   <sheetPr/>
   <dimension ref="A1:XFC11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1101,7 +1131,7 @@
     <col min="5" max="5" width="16.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1114,31 +1144,49 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="3" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="C2" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" ht="14.25" spans="1:16383">
       <c r="A3" s="4"/>
       <c r="B3" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="5"/>
@@ -17518,16 +17566,22 @@
       <c r="XFB3" s="5"/>
       <c r="XFC3" s="4"/>
     </row>
-    <row r="4" ht="14.25" spans="1:4">
+    <row r="4" ht="14.25" spans="1:6">
       <c r="A4" s="4"/>
       <c r="B4" s="5" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" ht="14.25" spans="1:3">
@@ -17581,17 +17635,19 @@
   <sheetPr/>
   <dimension ref="A1:XFC4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3"/>
   <cols>
     <col min="2" max="2" width="30.5" customWidth="1"/>
     <col min="3" max="3" width="30.125" customWidth="1"/>
+    <col min="5" max="5" width="18.375" customWidth="1"/>
+    <col min="6" max="6" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -17604,34 +17660,50 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="3" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" ht="14.25" spans="1:16383">
       <c r="A3" s="4"/>
       <c r="B3" s="5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="5"/>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
       <c r="G3" s="4"/>
       <c r="H3" s="5"/>
       <c r="I3" s="4"/>
@@ -34010,16 +34082,22 @@
       <c r="XFB3" s="5"/>
       <c r="XFC3" s="4"/>
     </row>
-    <row r="4" ht="14.25" spans="1:4">
+    <row r="4" ht="14.25" spans="1:6">
       <c r="A4" s="4"/>
       <c r="B4" s="5" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>